<commit_message>
Fixed an issue with the copying of data to the new infusion template.
I hadn't scrolled up when copying the samples.

Files checked in: DataRepo/example_data/AsaelR_13C-Valine+PI3Ki_flank-KPC_2021-12_isocorr_CN-corrected/TraceBase Animal and Sample Table Templates_AR.xlsx DataRepo/example_data/AsaelR_13C-Valine+PI3Ki_flank-KPC_2021-12_isocorr_CN-corrected/TraceBase Animal and Sample Table Templates_AR_old.xlsx
[skip ci]
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/AsaelR_13C-Valine+PI3Ki_flank-KPC_2021-12_isocorr_CN-corrected/TraceBase Animal and Sample Table Templates_AR.xlsx
+++ b/DataRepo/example_data/AsaelR_13C-Valine+PI3Ki_flank-KPC_2021-12_isocorr_CN-corrected/TraceBase Animal and Sample Table Templates_AR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/example_data/AsaelR_13C-Valine+PI3Ki_flank-KPC_2021-12_isocorr_CN-corrected/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E220BE1-8D41-DB45-A67C-F15980427A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC188A1E-C1E6-0547-A108-B1C48381DF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18800" yWindow="7300" windowWidth="32400" windowHeight="20140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18800" yWindow="7300" windowWidth="32400" windowHeight="20140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Animals" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Tissues" sheetId="4" r:id="rId4"/>
     <sheet name="Infusions" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -499,7 +499,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="247">
   <si>
     <t>Animal ID</t>
   </si>
@@ -999,6 +999,288 @@
   <si>
     <t>feces</t>
   </si>
+  <si>
+    <t>t0_a146</t>
+  </si>
+  <si>
+    <t>t0_a147</t>
+  </si>
+  <si>
+    <t>t0_a148</t>
+  </si>
+  <si>
+    <t>t0_a149</t>
+  </si>
+  <si>
+    <t>t0_a150</t>
+  </si>
+  <si>
+    <t>t0_a151</t>
+  </si>
+  <si>
+    <t>t90_a146</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>t90_a147</t>
+  </si>
+  <si>
+    <t>t90_a148</t>
+  </si>
+  <si>
+    <t>t90_a149</t>
+  </si>
+  <si>
+    <t>t90_a150</t>
+  </si>
+  <si>
+    <t>t120_a146</t>
+  </si>
+  <si>
+    <t>t120_a147</t>
+  </si>
+  <si>
+    <t>t120_a148</t>
+  </si>
+  <si>
+    <t>t120_a149</t>
+  </si>
+  <si>
+    <t>t120_a150</t>
+  </si>
+  <si>
+    <t>t120_a151</t>
+  </si>
+  <si>
+    <t>BAT_a147</t>
+  </si>
+  <si>
+    <t>BAT_a150</t>
+  </si>
+  <si>
+    <t>BAT_a151</t>
+  </si>
+  <si>
+    <t>Brain_a147</t>
+  </si>
+  <si>
+    <t>Brain_a150</t>
+  </si>
+  <si>
+    <t>Brain_a151</t>
+  </si>
+  <si>
+    <t>Colon_a147</t>
+  </si>
+  <si>
+    <t>Colon_a150</t>
+  </si>
+  <si>
+    <t>Colon_a151</t>
+  </si>
+  <si>
+    <t>Dia_a147</t>
+  </si>
+  <si>
+    <t>Dia_a150</t>
+  </si>
+  <si>
+    <t>Dia_a151</t>
+  </si>
+  <si>
+    <t>Feces_a147</t>
+  </si>
+  <si>
+    <t>Feces_a150</t>
+  </si>
+  <si>
+    <t>Feces_a151</t>
+  </si>
+  <si>
+    <t>Gastro_a147</t>
+  </si>
+  <si>
+    <t>Gastro_a150</t>
+  </si>
+  <si>
+    <t>Gastro_a151</t>
+  </si>
+  <si>
+    <t>gWAT_a147</t>
+  </si>
+  <si>
+    <t>gWAT_a150</t>
+  </si>
+  <si>
+    <t>gWAT_a151</t>
+  </si>
+  <si>
+    <t>Heart_a147</t>
+  </si>
+  <si>
+    <t>Heart_a150</t>
+  </si>
+  <si>
+    <t>Heart_a151</t>
+  </si>
+  <si>
+    <t>Kid_a147</t>
+  </si>
+  <si>
+    <t>Kid_a150</t>
+  </si>
+  <si>
+    <t>Kid_a151</t>
+  </si>
+  <si>
+    <t>Liv_a147</t>
+  </si>
+  <si>
+    <t>Liv_a150</t>
+  </si>
+  <si>
+    <t>Liv_a151</t>
+  </si>
+  <si>
+    <t>Lungs_a147</t>
+  </si>
+  <si>
+    <t>Lungs_a150</t>
+  </si>
+  <si>
+    <t>Lungs_a151</t>
+  </si>
+  <si>
+    <t>Pnc_a147</t>
+  </si>
+  <si>
+    <t>Pnc_a150</t>
+  </si>
+  <si>
+    <t>Pnc_a151</t>
+  </si>
+  <si>
+    <t>Quad_a147</t>
+  </si>
+  <si>
+    <t>Quad_a150</t>
+  </si>
+  <si>
+    <t>Quad_a151</t>
+  </si>
+  <si>
+    <t>SI_a147</t>
+  </si>
+  <si>
+    <t>SI_a150</t>
+  </si>
+  <si>
+    <t>SI_a151</t>
+  </si>
+  <si>
+    <t>Soleus_a147</t>
+  </si>
+  <si>
+    <t>Soleus_a150</t>
+  </si>
+  <si>
+    <t>Soleus_a151</t>
+  </si>
+  <si>
+    <t>Spleen_a147</t>
+  </si>
+  <si>
+    <t>Spleen_a150</t>
+  </si>
+  <si>
+    <t>Spleen_a151</t>
+  </si>
+  <si>
+    <t>Tumor_half_a147</t>
+  </si>
+  <si>
+    <t>Tumor_half_a150</t>
+  </si>
+  <si>
+    <t>Tumor_half_a151</t>
+  </si>
+  <si>
+    <t>Tumor_perif_a147</t>
+  </si>
+  <si>
+    <t>Tumor_perif_a150</t>
+  </si>
+  <si>
+    <t>Tumor_perif_a151</t>
+  </si>
+  <si>
+    <t>BAT_a146</t>
+  </si>
+  <si>
+    <t>BAT_a148</t>
+  </si>
+  <si>
+    <t>BAT_a149</t>
+  </si>
+  <si>
+    <t>Brain_a146</t>
+  </si>
+  <si>
+    <t>Brain_a148</t>
+  </si>
+  <si>
+    <t>Brain_a149</t>
+  </si>
+  <si>
+    <t>Colon_a146</t>
+  </si>
+  <si>
+    <t>Colon_a148</t>
+  </si>
+  <si>
+    <t>Colon_a149</t>
+  </si>
+  <si>
+    <t>Dia_146</t>
+  </si>
+  <si>
+    <t>Dia_148</t>
+  </si>
+  <si>
+    <t>Dia_149</t>
+  </si>
+  <si>
+    <t>Feces_a146</t>
+  </si>
+  <si>
+    <t>Feces_a148</t>
+  </si>
+  <si>
+    <t>Feces_a149</t>
+  </si>
+  <si>
+    <t>Gas_a146</t>
+  </si>
+  <si>
+    <t>Gas_a148</t>
+  </si>
+  <si>
+    <t>Gas_a149</t>
+  </si>
+  <si>
+    <t>gWAT_a146</t>
+  </si>
+  <si>
+    <t>gWAT_a148</t>
+  </si>
+  <si>
+    <t>gWAT_a149</t>
+  </si>
+  <si>
+    <t>Heart_a146</t>
+  </si>
 </sst>
 </file>
 
@@ -1180,7 +1462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -1227,6 +1509,7 @@
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6743,9 +7026,9 @@
   </sheetPr>
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:F35"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -6803,22 +7086,22 @@
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1">
       <c r="A2" s="28" t="s">
-        <v>113</v>
+        <v>153</v>
       </c>
       <c r="B2" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -6833,22 +7116,22 @@
     </row>
     <row r="3" spans="1:30" ht="15.75" customHeight="1">
       <c r="A3" s="28" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="B3" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C3" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -6863,22 +7146,22 @@
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1">
       <c r="A4" s="28" t="s">
-        <v>117</v>
+        <v>155</v>
       </c>
       <c r="B4" s="29">
-        <v>44531</v>
+        <v>44532</v>
       </c>
       <c r="C4" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -6893,7 +7176,7 @@
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1">
       <c r="A5" s="28" t="s">
-        <v>118</v>
+        <v>156</v>
       </c>
       <c r="B5" s="29">
         <v>44532</v>
@@ -6902,13 +7185,13 @@
         <v>114</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -6923,22 +7206,22 @@
     </row>
     <row r="6" spans="1:30" ht="15.75" customHeight="1">
       <c r="A6" s="28" t="s">
-        <v>119</v>
+        <v>157</v>
       </c>
       <c r="B6" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C6" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -6953,7 +7236,7 @@
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1">
       <c r="A7" s="28" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
       <c r="B7" s="29">
         <v>44531</v>
@@ -6962,13 +7245,13 @@
         <v>114</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -6983,22 +7266,22 @@
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1">
       <c r="A8" s="28" t="s">
-        <v>121</v>
+        <v>159</v>
       </c>
       <c r="B8" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C8" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -7013,22 +7296,22 @@
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1">
       <c r="A9" s="28" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
       <c r="B9" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C9" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -7043,22 +7326,22 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" customHeight="1">
       <c r="A10" s="28" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="B10" s="29">
-        <v>44531</v>
+        <v>44532</v>
       </c>
       <c r="C10" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -7073,7 +7356,7 @@
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1">
       <c r="A11" s="28" t="s">
-        <v>124</v>
+        <v>163</v>
       </c>
       <c r="B11" s="29">
         <v>44532</v>
@@ -7082,13 +7365,13 @@
         <v>114</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -7103,22 +7386,22 @@
     </row>
     <row r="12" spans="1:30" ht="15.75" customHeight="1">
       <c r="A12" s="28" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="B12" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
@@ -7133,7 +7416,7 @@
     </row>
     <row r="13" spans="1:30" ht="15.75" customHeight="1">
       <c r="A13" s="28" t="s">
-        <v>126</v>
+        <v>165</v>
       </c>
       <c r="B13" s="29">
         <v>44531</v>
@@ -7142,7 +7425,7 @@
         <v>114</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E13" s="30" t="s">
         <v>115</v>
@@ -7163,22 +7446,22 @@
     </row>
     <row r="14" spans="1:30" ht="15.75" customHeight="1">
       <c r="A14" s="28" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="B14" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C14" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E14" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F14" s="30" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -7193,7 +7476,7 @@
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1">
       <c r="A15" s="28" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
       <c r="B15" s="29">
         <v>44532</v>
@@ -7202,13 +7485,13 @@
         <v>114</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E15" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -7223,22 +7506,22 @@
     </row>
     <row r="16" spans="1:30" ht="15.75" customHeight="1">
       <c r="A16" s="28" t="s">
-        <v>129</v>
+        <v>168</v>
       </c>
       <c r="B16" s="29">
-        <v>44531</v>
+        <v>44532</v>
       </c>
       <c r="C16" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E16" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -7253,22 +7536,22 @@
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1">
       <c r="A17" s="28" t="s">
-        <v>130</v>
+        <v>169</v>
       </c>
       <c r="B17" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C17" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E17" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -7283,22 +7566,22 @@
     </row>
     <row r="18" spans="1:16" ht="15.75" customHeight="1">
       <c r="A18" s="28" t="s">
-        <v>131</v>
+        <v>170</v>
       </c>
       <c r="B18" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C18" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E18" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F18" s="30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -7313,7 +7596,7 @@
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1">
       <c r="A19" s="28" t="s">
-        <v>132</v>
+        <v>171</v>
       </c>
       <c r="B19" s="29">
         <v>44531</v>
@@ -7322,13 +7605,13 @@
         <v>114</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="E19" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F19" s="30" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -7343,22 +7626,22 @@
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1">
       <c r="A20" s="28" t="s">
-        <v>133</v>
+        <v>172</v>
       </c>
       <c r="B20" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C20" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="E20" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -7373,22 +7656,22 @@
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1">
       <c r="A21" s="28" t="s">
-        <v>134</v>
+        <v>173</v>
       </c>
       <c r="B21" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C21" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="E21" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F21" s="30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -7403,7 +7686,7 @@
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1">
       <c r="A22" s="28" t="s">
-        <v>135</v>
+        <v>174</v>
       </c>
       <c r="B22" s="29">
         <v>44531</v>
@@ -7412,13 +7695,13 @@
         <v>114</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="E22" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F22" s="30" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -7433,22 +7716,22 @@
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1">
       <c r="A23" s="28" t="s">
-        <v>136</v>
+        <v>175</v>
       </c>
       <c r="B23" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C23" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="E23" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -7463,22 +7746,22 @@
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1">
       <c r="A24" s="28" t="s">
-        <v>137</v>
+        <v>176</v>
       </c>
       <c r="B24" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C24" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="E24" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F24" s="30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
@@ -7493,7 +7776,7 @@
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1">
       <c r="A25" s="28" t="s">
-        <v>138</v>
+        <v>177</v>
       </c>
       <c r="B25" s="29">
         <v>44531</v>
@@ -7502,13 +7785,13 @@
         <v>114</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E25" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
@@ -7523,22 +7806,22 @@
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1">
       <c r="A26" s="28" t="s">
-        <v>139</v>
+        <v>178</v>
       </c>
       <c r="B26" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C26" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E26" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
@@ -7553,22 +7836,22 @@
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1">
       <c r="A27" s="28" t="s">
-        <v>140</v>
+        <v>179</v>
       </c>
       <c r="B27" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E27" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
@@ -7583,7 +7866,7 @@
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1">
       <c r="A28" s="28" t="s">
-        <v>141</v>
+        <v>180</v>
       </c>
       <c r="B28" s="29">
         <v>44531</v>
@@ -7592,13 +7875,13 @@
         <v>114</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="E28" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F28" s="30" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
@@ -7613,22 +7896,22 @@
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1">
       <c r="A29" s="28" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
       <c r="B29" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C29" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="E29" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F29" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
@@ -7643,22 +7926,22 @@
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1">
       <c r="A30" s="28" t="s">
-        <v>143</v>
+        <v>182</v>
       </c>
       <c r="B30" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C30" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="E30" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
@@ -7673,7 +7956,7 @@
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1">
       <c r="A31" s="28" t="s">
-        <v>144</v>
+        <v>183</v>
       </c>
       <c r="B31" s="29">
         <v>44531</v>
@@ -7682,13 +7965,13 @@
         <v>114</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>77</v>
+        <v>152</v>
       </c>
       <c r="E31" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
@@ -7703,22 +7986,22 @@
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1">
       <c r="A32" s="28" t="s">
-        <v>145</v>
+        <v>184</v>
       </c>
       <c r="B32" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C32" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>77</v>
+        <v>152</v>
       </c>
       <c r="E32" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F32" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
@@ -7733,22 +8016,22 @@
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1">
       <c r="A33" s="28" t="s">
-        <v>146</v>
+        <v>185</v>
       </c>
       <c r="B33" s="29">
-        <v>44532</v>
+        <v>44531</v>
       </c>
       <c r="C33" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>77</v>
+        <v>152</v>
       </c>
       <c r="E33" s="30" t="s">
         <v>115</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
@@ -7762,8 +8045,8 @@
       <c r="P33" s="5"/>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A34" s="31" t="s">
-        <v>147</v>
+      <c r="A34" s="28" t="s">
+        <v>186</v>
       </c>
       <c r="B34" s="29">
         <v>44531</v>
@@ -7772,13 +8055,13 @@
         <v>114</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>148</v>
+        <v>115</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
@@ -7792,8 +8075,8 @@
       <c r="P34" s="5"/>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A35" s="31" t="s">
-        <v>149</v>
+      <c r="A35" s="28" t="s">
+        <v>187</v>
       </c>
       <c r="B35" s="29">
         <v>44531</v>
@@ -7802,13 +8085,13 @@
         <v>114</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>148</v>
+        <v>115</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
@@ -7822,12 +8105,24 @@
       <c r="P35" s="5"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A36" s="5"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
+      <c r="A36" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="B36" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F36" s="30" t="s">
+        <v>101</v>
+      </c>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
@@ -7840,12 +8135,24 @@
       <c r="P36" s="5"/>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A37" s="5"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
+      <c r="A37" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="B37" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F37" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
@@ -7858,12 +8165,24 @@
       <c r="P37" s="5"/>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A38" s="5"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
+      <c r="A38" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="B38" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F38" s="30" t="s">
+        <v>100</v>
+      </c>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
@@ -7876,12 +8195,24 @@
       <c r="P38" s="5"/>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A39" s="5"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
+      <c r="A39" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="B39" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39" s="30" t="s">
+        <v>101</v>
+      </c>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -7894,12 +8225,24 @@
       <c r="P39" s="5"/>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A40" s="5"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
+      <c r="A40" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="B40" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E40" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F40" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -7912,12 +8255,24 @@
       <c r="P40" s="5"/>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A41" s="5"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
+      <c r="A41" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="B41" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" s="30" t="s">
+        <v>100</v>
+      </c>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
@@ -7930,12 +8285,24 @@
       <c r="P41" s="5"/>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A42" s="5"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
+      <c r="A42" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="B42" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F42" s="30" t="s">
+        <v>101</v>
+      </c>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
@@ -7948,12 +8315,24 @@
       <c r="P42" s="5"/>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A43" s="5"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
+      <c r="A43" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="B43" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E43" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F43" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
@@ -7966,12 +8345,24 @@
       <c r="P43" s="5"/>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A44" s="5"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
+      <c r="A44" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="B44" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C44" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E44" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F44" s="30" t="s">
+        <v>100</v>
+      </c>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
@@ -7984,12 +8375,24 @@
       <c r="P44" s="5"/>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A45" s="5"/>
-      <c r="B45" s="10"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
+      <c r="A45" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="B45" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E45" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F45" s="30" t="s">
+        <v>101</v>
+      </c>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
@@ -8002,12 +8405,24 @@
       <c r="P45" s="5"/>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A46" s="5"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
+      <c r="A46" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="B46" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C46" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F46" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
@@ -8020,12 +8435,24 @@
       <c r="P46" s="5"/>
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A47" s="5"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
+      <c r="A47" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="B47" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C47" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F47" s="30" t="s">
+        <v>100</v>
+      </c>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
@@ -8038,12 +8465,24 @@
       <c r="P47" s="5"/>
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A48" s="5"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
+      <c r="A48" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="B48" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E48" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F48" s="30" t="s">
+        <v>101</v>
+      </c>
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
@@ -8056,12 +8495,24 @@
       <c r="P48" s="5"/>
     </row>
     <row r="49" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A49" s="5"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
+      <c r="A49" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="B49" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E49" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F49" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
@@ -8074,12 +8525,24 @@
       <c r="P49" s="5"/>
     </row>
     <row r="50" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A50" s="5"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
+      <c r="A50" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="B50" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C50" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F50" s="30" t="s">
+        <v>100</v>
+      </c>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
@@ -8092,12 +8555,24 @@
       <c r="P50" s="5"/>
     </row>
     <row r="51" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A51" s="5"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
+      <c r="A51" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="B51" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C51" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E51" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F51" s="30" t="s">
+        <v>101</v>
+      </c>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
@@ -8110,12 +8585,24 @@
       <c r="P51" s="5"/>
     </row>
     <row r="52" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A52" s="5"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
+      <c r="A52" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="B52" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C52" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E52" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F52" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
@@ -8128,12 +8615,24 @@
       <c r="P52" s="5"/>
     </row>
     <row r="53" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A53" s="5"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
+      <c r="A53" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="B53" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C53" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E53" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F53" s="30" t="s">
+        <v>100</v>
+      </c>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
@@ -8146,12 +8645,24 @@
       <c r="P53" s="5"/>
     </row>
     <row r="54" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A54" s="5"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
+      <c r="A54" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="B54" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E54" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F54" s="30" t="s">
+        <v>101</v>
+      </c>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
@@ -8164,12 +8675,24 @@
       <c r="P54" s="5"/>
     </row>
     <row r="55" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A55" s="5"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
+      <c r="A55" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="B55" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C55" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E55" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F55" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
@@ -8182,12 +8705,24 @@
       <c r="P55" s="5"/>
     </row>
     <row r="56" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A56" s="5"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
+      <c r="A56" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="B56" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C56" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D56" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E56" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F56" s="30" t="s">
+        <v>100</v>
+      </c>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
@@ -8200,12 +8735,24 @@
       <c r="P56" s="5"/>
     </row>
     <row r="57" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A57" s="5"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
+      <c r="A57" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="B57" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C57" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D57" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E57" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F57" s="30" t="s">
+        <v>101</v>
+      </c>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
@@ -8218,12 +8765,24 @@
       <c r="P57" s="5"/>
     </row>
     <row r="58" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A58" s="5"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
+      <c r="A58" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="B58" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C58" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D58" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E58" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F58" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
@@ -8236,12 +8795,24 @@
       <c r="P58" s="5"/>
     </row>
     <row r="59" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A59" s="5"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
+      <c r="A59" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="B59" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C59" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D59" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E59" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F59" s="30" t="s">
+        <v>100</v>
+      </c>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
@@ -8254,12 +8825,24 @@
       <c r="P59" s="5"/>
     </row>
     <row r="60" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A60" s="5"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
+      <c r="A60" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="B60" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C60" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D60" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E60" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F60" s="30" t="s">
+        <v>101</v>
+      </c>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
@@ -8272,12 +8855,24 @@
       <c r="P60" s="5"/>
     </row>
     <row r="61" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A61" s="5"/>
-      <c r="B61" s="10"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
+      <c r="A61" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="B61" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C61" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D61" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E61" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F61" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
@@ -8290,12 +8885,24 @@
       <c r="P61" s="5"/>
     </row>
     <row r="62" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A62" s="5"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
+      <c r="A62" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="B62" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C62" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D62" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E62" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F62" s="30" t="s">
+        <v>100</v>
+      </c>
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
@@ -8308,12 +8915,24 @@
       <c r="P62" s="5"/>
     </row>
     <row r="63" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A63" s="5"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
+      <c r="A63" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="B63" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C63" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D63" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E63" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F63" s="30" t="s">
+        <v>101</v>
+      </c>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
@@ -8326,12 +8945,24 @@
       <c r="P63" s="5"/>
     </row>
     <row r="64" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A64" s="5"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
+      <c r="A64" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="B64" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C64" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D64" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E64" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F64" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
@@ -8344,12 +8975,24 @@
       <c r="P64" s="5"/>
     </row>
     <row r="65" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A65" s="5"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
+      <c r="A65" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B65" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C65" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D65" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E65" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F65" s="30" t="s">
+        <v>100</v>
+      </c>
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
@@ -8362,12 +9005,24 @@
       <c r="P65" s="5"/>
     </row>
     <row r="66" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A66" s="5"/>
-      <c r="B66" s="10"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
+      <c r="A66" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="B66" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C66" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D66" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E66" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F66" s="30" t="s">
+        <v>101</v>
+      </c>
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
@@ -8380,12 +9035,24 @@
       <c r="P66" s="5"/>
     </row>
     <row r="67" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A67" s="5"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
+      <c r="A67" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="B67" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C67" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D67" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E67" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F67" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
@@ -8398,12 +9065,24 @@
       <c r="P67" s="5"/>
     </row>
     <row r="68" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A68" s="5"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
+      <c r="A68" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="B68" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C68" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D68" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E68" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F68" s="30" t="s">
+        <v>100</v>
+      </c>
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
@@ -8416,12 +9095,24 @@
       <c r="P68" s="5"/>
     </row>
     <row r="69" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A69" s="5"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
+      <c r="A69" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="B69" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C69" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D69" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E69" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F69" s="30" t="s">
+        <v>101</v>
+      </c>
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
@@ -8434,12 +9125,24 @@
       <c r="P69" s="5"/>
     </row>
     <row r="70" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A70" s="5"/>
-      <c r="B70" s="10"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
+      <c r="A70" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="B70" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C70" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D70" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E70" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F70" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="G70" s="5"/>
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
@@ -8452,12 +9155,24 @@
       <c r="P70" s="5"/>
     </row>
     <row r="71" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A71" s="5"/>
-      <c r="B71" s="10"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
+      <c r="A71" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="B71" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C71" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D71" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E71" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F71" s="30" t="s">
+        <v>100</v>
+      </c>
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
@@ -8470,12 +9185,24 @@
       <c r="P71" s="5"/>
     </row>
     <row r="72" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A72" s="5"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
+      <c r="A72" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="B72" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C72" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D72" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E72" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F72" s="30" t="s">
+        <v>101</v>
+      </c>
       <c r="G72" s="5"/>
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
@@ -8488,12 +9215,24 @@
       <c r="P72" s="5"/>
     </row>
     <row r="73" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A73" s="5"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
+      <c r="A73" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="B73" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C73" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D73" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E73" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F73" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
@@ -8506,12 +9245,24 @@
       <c r="P73" s="5"/>
     </row>
     <row r="74" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A74" s="5"/>
-      <c r="B74" s="10"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
+      <c r="A74" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="B74" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C74" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D74" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E74" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F74" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
@@ -8524,12 +9275,24 @@
       <c r="P74" s="5"/>
     </row>
     <row r="75" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A75" s="5"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
+      <c r="A75" s="34" t="s">
+        <v>227</v>
+      </c>
+      <c r="B75" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C75" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D75" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E75" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F75" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
@@ -8542,12 +9305,24 @@
       <c r="P75" s="5"/>
     </row>
     <row r="76" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A76" s="5"/>
-      <c r="B76" s="10"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
+      <c r="A76" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="B76" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C76" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D76" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E76" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F76" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
@@ -8560,12 +9335,24 @@
       <c r="P76" s="5"/>
     </row>
     <row r="77" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A77" s="5"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="5"/>
+      <c r="A77" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="B77" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C77" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D77" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E77" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F77" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
@@ -8578,12 +9365,24 @@
       <c r="P77" s="5"/>
     </row>
     <row r="78" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A78" s="5"/>
-      <c r="B78" s="10"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
+      <c r="A78" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="B78" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C78" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D78" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E78" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F78" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G78" s="5"/>
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
@@ -8596,12 +9395,24 @@
       <c r="P78" s="5"/>
     </row>
     <row r="79" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A79" s="5"/>
-      <c r="B79" s="10"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5"/>
-      <c r="F79" s="5"/>
+      <c r="A79" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="B79" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C79" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D79" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E79" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F79" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G79" s="5"/>
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
@@ -8614,12 +9425,24 @@
       <c r="P79" s="5"/>
     </row>
     <row r="80" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A80" s="5"/>
-      <c r="B80" s="10"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="5"/>
+      <c r="A80" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="B80" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C80" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D80" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E80" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F80" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G80" s="5"/>
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
@@ -8632,12 +9455,24 @@
       <c r="P80" s="5"/>
     </row>
     <row r="81" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A81" s="5"/>
-      <c r="B81" s="10"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="5"/>
+      <c r="A81" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="B81" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C81" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D81" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E81" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F81" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G81" s="5"/>
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
@@ -8650,12 +9485,24 @@
       <c r="P81" s="5"/>
     </row>
     <row r="82" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A82" s="5"/>
-      <c r="B82" s="10"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="5"/>
+      <c r="A82" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="B82" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C82" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D82" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E82" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F82" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G82" s="5"/>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
@@ -8668,12 +9515,24 @@
       <c r="P82" s="5"/>
     </row>
     <row r="83" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A83" s="5"/>
-      <c r="B83" s="10"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
+      <c r="A83" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="B83" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C83" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D83" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E83" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F83" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
@@ -8685,13 +9544,25 @@
       <c r="O83" s="5"/>
       <c r="P83" s="5"/>
     </row>
-    <row r="84" spans="1:16" ht="13">
-      <c r="A84" s="5"/>
-      <c r="B84" s="10"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
+    <row r="84" spans="1:16" ht="15">
+      <c r="A84" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="B84" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C84" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D84" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E84" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F84" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
@@ -8703,13 +9574,25 @@
       <c r="O84" s="5"/>
       <c r="P84" s="5"/>
     </row>
-    <row r="85" spans="1:16" ht="13">
-      <c r="A85" s="5"/>
-      <c r="B85" s="10"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5"/>
-      <c r="F85" s="5"/>
+    <row r="85" spans="1:16" ht="15">
+      <c r="A85" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="B85" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C85" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D85" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="E85" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F85" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G85" s="5"/>
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
@@ -8721,13 +9604,25 @@
       <c r="O85" s="5"/>
       <c r="P85" s="5"/>
     </row>
-    <row r="86" spans="1:16" ht="13">
-      <c r="A86" s="5"/>
-      <c r="B86" s="10"/>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
-      <c r="E86" s="5"/>
-      <c r="F86" s="5"/>
+    <row r="86" spans="1:16" ht="15">
+      <c r="A86" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="B86" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C86" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D86" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="E86" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F86" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
@@ -8739,13 +9634,25 @@
       <c r="O86" s="5"/>
       <c r="P86" s="5"/>
     </row>
-    <row r="87" spans="1:16" ht="13">
-      <c r="A87" s="5"/>
-      <c r="B87" s="10"/>
-      <c r="C87" s="5"/>
-      <c r="D87" s="5"/>
-      <c r="E87" s="5"/>
-      <c r="F87" s="5"/>
+    <row r="87" spans="1:16" ht="15">
+      <c r="A87" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="B87" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C87" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D87" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="E87" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F87" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G87" s="5"/>
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
@@ -8757,13 +9664,25 @@
       <c r="O87" s="5"/>
       <c r="P87" s="5"/>
     </row>
-    <row r="88" spans="1:16" ht="13">
-      <c r="A88" s="5"/>
-      <c r="B88" s="10"/>
-      <c r="C88" s="5"/>
-      <c r="D88" s="5"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5"/>
+    <row r="88" spans="1:16" ht="15">
+      <c r="A88" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="B88" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C88" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D88" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E88" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F88" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G88" s="5"/>
       <c r="H88" s="5"/>
       <c r="I88" s="5"/>
@@ -8775,13 +9694,25 @@
       <c r="O88" s="5"/>
       <c r="P88" s="5"/>
     </row>
-    <row r="89" spans="1:16" ht="13">
-      <c r="A89" s="5"/>
-      <c r="B89" s="10"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
+    <row r="89" spans="1:16" ht="15">
+      <c r="A89" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="B89" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C89" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D89" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E89" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F89" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G89" s="5"/>
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
@@ -8793,13 +9724,25 @@
       <c r="O89" s="5"/>
       <c r="P89" s="5"/>
     </row>
-    <row r="90" spans="1:16" ht="13">
-      <c r="A90" s="5"/>
-      <c r="B90" s="10"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
+    <row r="90" spans="1:16" ht="15">
+      <c r="A90" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="B90" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C90" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D90" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E90" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F90" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
@@ -8811,13 +9754,25 @@
       <c r="O90" s="5"/>
       <c r="P90" s="5"/>
     </row>
-    <row r="91" spans="1:16" ht="13">
-      <c r="A91" s="5"/>
-      <c r="B91" s="10"/>
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
+    <row r="91" spans="1:16" ht="15">
+      <c r="A91" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B91" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C91" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D91" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E91" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F91" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
@@ -8829,13 +9784,25 @@
       <c r="O91" s="5"/>
       <c r="P91" s="5"/>
     </row>
-    <row r="92" spans="1:16" ht="13">
-      <c r="A92" s="5"/>
-      <c r="B92" s="10"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
+    <row r="92" spans="1:16" ht="15">
+      <c r="A92" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="B92" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C92" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D92" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E92" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F92" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G92" s="5"/>
       <c r="H92" s="5"/>
       <c r="I92" s="5"/>
@@ -8847,13 +9814,25 @@
       <c r="O92" s="5"/>
       <c r="P92" s="5"/>
     </row>
-    <row r="93" spans="1:16" ht="13">
-      <c r="A93" s="5"/>
-      <c r="B93" s="10"/>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="F93" s="5"/>
+    <row r="93" spans="1:16" ht="15">
+      <c r="A93" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="B93" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C93" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D93" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E93" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F93" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G93" s="5"/>
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
@@ -8865,13 +9844,25 @@
       <c r="O93" s="5"/>
       <c r="P93" s="5"/>
     </row>
-    <row r="94" spans="1:16" ht="13">
-      <c r="A94" s="5"/>
-      <c r="B94" s="10"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
+    <row r="94" spans="1:16" ht="15">
+      <c r="A94" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="B94" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C94" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D94" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E94" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F94" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G94" s="5"/>
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
@@ -8883,13 +9874,25 @@
       <c r="O94" s="5"/>
       <c r="P94" s="5"/>
     </row>
-    <row r="95" spans="1:16" ht="13">
-      <c r="A95" s="5"/>
-      <c r="B95" s="10"/>
-      <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="5"/>
+    <row r="95" spans="1:16" ht="15">
+      <c r="A95" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B95" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C95" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D95" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E95" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F95" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G95" s="5"/>
       <c r="H95" s="5"/>
       <c r="I95" s="5"/>
@@ -8901,13 +9904,25 @@
       <c r="O95" s="5"/>
       <c r="P95" s="5"/>
     </row>
-    <row r="96" spans="1:16" ht="13">
-      <c r="A96" s="5"/>
-      <c r="B96" s="10"/>
-      <c r="C96" s="5"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="5"/>
-      <c r="F96" s="5"/>
+    <row r="96" spans="1:16" ht="15">
+      <c r="A96" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B96" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C96" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D96" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E96" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F96" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G96" s="5"/>
       <c r="H96" s="5"/>
       <c r="I96" s="5"/>
@@ -8919,13 +9934,25 @@
       <c r="O96" s="5"/>
       <c r="P96" s="5"/>
     </row>
-    <row r="97" spans="1:16" ht="13">
-      <c r="A97" s="5"/>
-      <c r="B97" s="10"/>
-      <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="5"/>
+    <row r="97" spans="1:16" ht="15">
+      <c r="A97" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="B97" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C97" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D97" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E97" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F97" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G97" s="5"/>
       <c r="H97" s="5"/>
       <c r="I97" s="5"/>
@@ -8937,13 +9964,25 @@
       <c r="O97" s="5"/>
       <c r="P97" s="5"/>
     </row>
-    <row r="98" spans="1:16" ht="13">
-      <c r="A98" s="5"/>
-      <c r="B98" s="10"/>
-      <c r="C98" s="5"/>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
+    <row r="98" spans="1:16" ht="15">
+      <c r="A98" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B98" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C98" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D98" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E98" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F98" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G98" s="5"/>
       <c r="H98" s="5"/>
       <c r="I98" s="5"/>
@@ -8955,13 +9994,25 @@
       <c r="O98" s="5"/>
       <c r="P98" s="5"/>
     </row>
-    <row r="99" spans="1:16" ht="13">
-      <c r="A99" s="5"/>
-      <c r="B99" s="10"/>
-      <c r="C99" s="5"/>
-      <c r="D99" s="5"/>
-      <c r="E99" s="5"/>
-      <c r="F99" s="5"/>
+    <row r="99" spans="1:16" ht="15">
+      <c r="A99" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B99" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C99" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D99" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E99" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F99" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G99" s="5"/>
       <c r="H99" s="5"/>
       <c r="I99" s="5"/>
@@ -8973,13 +10024,25 @@
       <c r="O99" s="5"/>
       <c r="P99" s="5"/>
     </row>
-    <row r="100" spans="1:16" ht="13">
-      <c r="A100" s="5"/>
-      <c r="B100" s="10"/>
-      <c r="C100" s="5"/>
-      <c r="D100" s="5"/>
-      <c r="E100" s="5"/>
-      <c r="F100" s="5"/>
+    <row r="100" spans="1:16" ht="15">
+      <c r="A100" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B100" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C100" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D100" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E100" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F100" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G100" s="5"/>
       <c r="H100" s="5"/>
       <c r="I100" s="5"/>
@@ -8991,13 +10054,25 @@
       <c r="O100" s="5"/>
       <c r="P100" s="5"/>
     </row>
-    <row r="101" spans="1:16" ht="13">
-      <c r="A101" s="5"/>
-      <c r="B101" s="10"/>
-      <c r="C101" s="5"/>
-      <c r="D101" s="5"/>
-      <c r="E101" s="5"/>
-      <c r="F101" s="5"/>
+    <row r="101" spans="1:16" ht="15">
+      <c r="A101" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B101" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C101" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D101" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E101" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F101" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G101" s="5"/>
       <c r="H101" s="5"/>
       <c r="I101" s="5"/>
@@ -9009,13 +10084,25 @@
       <c r="O101" s="5"/>
       <c r="P101" s="5"/>
     </row>
-    <row r="102" spans="1:16" ht="13">
-      <c r="A102" s="5"/>
-      <c r="B102" s="10"/>
-      <c r="C102" s="5"/>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="5"/>
+    <row r="102" spans="1:16" ht="15">
+      <c r="A102" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B102" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C102" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D102" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E102" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F102" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G102" s="5"/>
       <c r="H102" s="5"/>
       <c r="I102" s="5"/>
@@ -9027,13 +10114,25 @@
       <c r="O102" s="5"/>
       <c r="P102" s="5"/>
     </row>
-    <row r="103" spans="1:16" ht="13">
-      <c r="A103" s="5"/>
-      <c r="B103" s="10"/>
-      <c r="C103" s="5"/>
-      <c r="D103" s="5"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="5"/>
+    <row r="103" spans="1:16" ht="15">
+      <c r="A103" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B103" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C103" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D103" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E103" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F103" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G103" s="5"/>
       <c r="H103" s="5"/>
       <c r="I103" s="5"/>
@@ -9045,13 +10144,25 @@
       <c r="O103" s="5"/>
       <c r="P103" s="5"/>
     </row>
-    <row r="104" spans="1:16" ht="13">
-      <c r="A104" s="5"/>
-      <c r="B104" s="10"/>
-      <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="5"/>
+    <row r="104" spans="1:16" ht="15">
+      <c r="A104" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B104" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C104" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D104" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E104" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F104" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G104" s="5"/>
       <c r="H104" s="5"/>
       <c r="I104" s="5"/>
@@ -9063,13 +10174,25 @@
       <c r="O104" s="5"/>
       <c r="P104" s="5"/>
     </row>
-    <row r="105" spans="1:16" ht="13">
-      <c r="A105" s="5"/>
-      <c r="B105" s="10"/>
-      <c r="C105" s="5"/>
-      <c r="D105" s="5"/>
-      <c r="E105" s="5"/>
-      <c r="F105" s="5"/>
+    <row r="105" spans="1:16" ht="15">
+      <c r="A105" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="B105" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C105" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D105" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E105" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F105" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G105" s="5"/>
       <c r="H105" s="5"/>
       <c r="I105" s="5"/>
@@ -9081,13 +10204,25 @@
       <c r="O105" s="5"/>
       <c r="P105" s="5"/>
     </row>
-    <row r="106" spans="1:16" ht="13">
-      <c r="A106" s="5"/>
-      <c r="B106" s="10"/>
-      <c r="C106" s="5"/>
-      <c r="D106" s="5"/>
-      <c r="E106" s="5"/>
-      <c r="F106" s="5"/>
+    <row r="106" spans="1:16" ht="15">
+      <c r="A106" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="B106" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C106" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D106" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E106" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F106" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G106" s="5"/>
       <c r="H106" s="5"/>
       <c r="I106" s="5"/>
@@ -9099,13 +10234,25 @@
       <c r="O106" s="5"/>
       <c r="P106" s="5"/>
     </row>
-    <row r="107" spans="1:16" ht="13">
-      <c r="A107" s="5"/>
-      <c r="B107" s="10"/>
-      <c r="C107" s="5"/>
-      <c r="D107" s="5"/>
-      <c r="E107" s="5"/>
-      <c r="F107" s="5"/>
+    <row r="107" spans="1:16" ht="15">
+      <c r="A107" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B107" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C107" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D107" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E107" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F107" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G107" s="5"/>
       <c r="H107" s="5"/>
       <c r="I107" s="5"/>
@@ -9117,13 +10264,25 @@
       <c r="O107" s="5"/>
       <c r="P107" s="5"/>
     </row>
-    <row r="108" spans="1:16" ht="13">
-      <c r="A108" s="5"/>
-      <c r="B108" s="10"/>
-      <c r="C108" s="5"/>
-      <c r="D108" s="5"/>
-      <c r="E108" s="5"/>
-      <c r="F108" s="5"/>
+    <row r="108" spans="1:16" ht="15">
+      <c r="A108" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B108" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C108" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D108" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E108" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F108" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G108" s="5"/>
       <c r="H108" s="5"/>
       <c r="I108" s="5"/>
@@ -9135,13 +10294,25 @@
       <c r="O108" s="5"/>
       <c r="P108" s="5"/>
     </row>
-    <row r="109" spans="1:16" ht="13">
-      <c r="A109" s="5"/>
-      <c r="B109" s="10"/>
-      <c r="C109" s="5"/>
-      <c r="D109" s="5"/>
-      <c r="E109" s="5"/>
-      <c r="F109" s="5"/>
+    <row r="109" spans="1:16" ht="15">
+      <c r="A109" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="B109" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C109" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D109" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E109" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F109" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G109" s="5"/>
       <c r="H109" s="5"/>
       <c r="I109" s="5"/>
@@ -9153,13 +10324,25 @@
       <c r="O109" s="5"/>
       <c r="P109" s="5"/>
     </row>
-    <row r="110" spans="1:16" ht="13">
-      <c r="A110" s="5"/>
-      <c r="B110" s="10"/>
-      <c r="C110" s="5"/>
-      <c r="D110" s="5"/>
-      <c r="E110" s="5"/>
-      <c r="F110" s="5"/>
+    <row r="110" spans="1:16" ht="15">
+      <c r="A110" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="B110" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C110" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D110" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E110" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F110" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G110" s="5"/>
       <c r="H110" s="5"/>
       <c r="I110" s="5"/>
@@ -9171,13 +10354,25 @@
       <c r="O110" s="5"/>
       <c r="P110" s="5"/>
     </row>
-    <row r="111" spans="1:16" ht="13">
-      <c r="A111" s="5"/>
-      <c r="B111" s="10"/>
-      <c r="C111" s="5"/>
-      <c r="D111" s="5"/>
-      <c r="E111" s="5"/>
-      <c r="F111" s="5"/>
+    <row r="111" spans="1:16" ht="15">
+      <c r="A111" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="B111" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C111" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D111" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E111" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F111" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G111" s="5"/>
       <c r="H111" s="5"/>
       <c r="I111" s="5"/>
@@ -9189,13 +10384,25 @@
       <c r="O111" s="5"/>
       <c r="P111" s="5"/>
     </row>
-    <row r="112" spans="1:16" ht="13">
-      <c r="A112" s="5"/>
-      <c r="B112" s="10"/>
-      <c r="C112" s="5"/>
-      <c r="D112" s="5"/>
-      <c r="E112" s="5"/>
-      <c r="F112" s="5"/>
+    <row r="112" spans="1:16" ht="15">
+      <c r="A112" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B112" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C112" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D112" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E112" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F112" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G112" s="5"/>
       <c r="H112" s="5"/>
       <c r="I112" s="5"/>
@@ -9207,13 +10414,25 @@
       <c r="O112" s="5"/>
       <c r="P112" s="5"/>
     </row>
-    <row r="113" spans="1:16" ht="13">
-      <c r="A113" s="5"/>
-      <c r="B113" s="10"/>
-      <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
-      <c r="E113" s="5"/>
-      <c r="F113" s="5"/>
+    <row r="113" spans="1:16" ht="15">
+      <c r="A113" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B113" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C113" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D113" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E113" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F113" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G113" s="5"/>
       <c r="H113" s="5"/>
       <c r="I113" s="5"/>
@@ -9225,13 +10444,25 @@
       <c r="O113" s="5"/>
       <c r="P113" s="5"/>
     </row>
-    <row r="114" spans="1:16" ht="13">
-      <c r="A114" s="5"/>
-      <c r="B114" s="10"/>
-      <c r="C114" s="5"/>
-      <c r="D114" s="5"/>
-      <c r="E114" s="5"/>
-      <c r="F114" s="5"/>
+    <row r="114" spans="1:16" ht="15">
+      <c r="A114" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="B114" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C114" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D114" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E114" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F114" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G114" s="5"/>
       <c r="H114" s="5"/>
       <c r="I114" s="5"/>
@@ -9243,13 +10474,25 @@
       <c r="O114" s="5"/>
       <c r="P114" s="5"/>
     </row>
-    <row r="115" spans="1:16" ht="13">
-      <c r="A115" s="5"/>
-      <c r="B115" s="10"/>
-      <c r="C115" s="5"/>
-      <c r="D115" s="5"/>
-      <c r="E115" s="5"/>
-      <c r="F115" s="5"/>
+    <row r="115" spans="1:16" ht="15">
+      <c r="A115" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="B115" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C115" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D115" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E115" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F115" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G115" s="5"/>
       <c r="H115" s="5"/>
       <c r="I115" s="5"/>
@@ -9261,13 +10504,25 @@
       <c r="O115" s="5"/>
       <c r="P115" s="5"/>
     </row>
-    <row r="116" spans="1:16" ht="13">
-      <c r="A116" s="5"/>
-      <c r="B116" s="10"/>
-      <c r="C116" s="5"/>
-      <c r="D116" s="5"/>
-      <c r="E116" s="5"/>
-      <c r="F116" s="5"/>
+    <row r="116" spans="1:16" ht="15">
+      <c r="A116" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="B116" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C116" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D116" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E116" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F116" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G116" s="5"/>
       <c r="H116" s="5"/>
       <c r="I116" s="5"/>
@@ -9279,13 +10534,25 @@
       <c r="O116" s="5"/>
       <c r="P116" s="5"/>
     </row>
-    <row r="117" spans="1:16" ht="13">
-      <c r="A117" s="5"/>
-      <c r="B117" s="10"/>
-      <c r="C117" s="5"/>
-      <c r="D117" s="5"/>
-      <c r="E117" s="5"/>
-      <c r="F117" s="5"/>
+    <row r="117" spans="1:16" ht="15">
+      <c r="A117" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="B117" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C117" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D117" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E117" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F117" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G117" s="5"/>
       <c r="H117" s="5"/>
       <c r="I117" s="5"/>
@@ -9297,13 +10564,25 @@
       <c r="O117" s="5"/>
       <c r="P117" s="5"/>
     </row>
-    <row r="118" spans="1:16" ht="13">
-      <c r="A118" s="5"/>
-      <c r="B118" s="10"/>
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
-      <c r="E118" s="5"/>
-      <c r="F118" s="5"/>
+    <row r="118" spans="1:16" ht="15">
+      <c r="A118" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="B118" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C118" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D118" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E118" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F118" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G118" s="5"/>
       <c r="H118" s="5"/>
       <c r="I118" s="5"/>
@@ -9315,13 +10594,25 @@
       <c r="O118" s="5"/>
       <c r="P118" s="5"/>
     </row>
-    <row r="119" spans="1:16" ht="13">
-      <c r="A119" s="5"/>
-      <c r="B119" s="10"/>
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
-      <c r="E119" s="5"/>
-      <c r="F119" s="5"/>
+    <row r="119" spans="1:16" ht="15">
+      <c r="A119" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="B119" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C119" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D119" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E119" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F119" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G119" s="5"/>
       <c r="H119" s="5"/>
       <c r="I119" s="5"/>
@@ -9333,13 +10624,25 @@
       <c r="O119" s="5"/>
       <c r="P119" s="5"/>
     </row>
-    <row r="120" spans="1:16" ht="13">
-      <c r="A120" s="5"/>
-      <c r="B120" s="10"/>
-      <c r="C120" s="5"/>
-      <c r="D120" s="5"/>
-      <c r="E120" s="5"/>
-      <c r="F120" s="5"/>
+    <row r="120" spans="1:16" ht="15">
+      <c r="A120" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="B120" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C120" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D120" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E120" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F120" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G120" s="5"/>
       <c r="H120" s="5"/>
       <c r="I120" s="5"/>
@@ -9351,13 +10654,25 @@
       <c r="O120" s="5"/>
       <c r="P120" s="5"/>
     </row>
-    <row r="121" spans="1:16" ht="13">
-      <c r="A121" s="5"/>
-      <c r="B121" s="10"/>
-      <c r="C121" s="5"/>
-      <c r="D121" s="5"/>
-      <c r="E121" s="5"/>
-      <c r="F121" s="5"/>
+    <row r="121" spans="1:16" ht="15">
+      <c r="A121" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="B121" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C121" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D121" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E121" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F121" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G121" s="5"/>
       <c r="H121" s="5"/>
       <c r="I121" s="5"/>
@@ -9369,13 +10684,25 @@
       <c r="O121" s="5"/>
       <c r="P121" s="5"/>
     </row>
-    <row r="122" spans="1:16" ht="13">
-      <c r="A122" s="5"/>
-      <c r="B122" s="10"/>
-      <c r="C122" s="5"/>
-      <c r="D122" s="5"/>
-      <c r="E122" s="5"/>
-      <c r="F122" s="5"/>
+    <row r="122" spans="1:16" ht="15">
+      <c r="A122" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="B122" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C122" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D122" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E122" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F122" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G122" s="5"/>
       <c r="H122" s="5"/>
       <c r="I122" s="5"/>
@@ -9387,13 +10714,25 @@
       <c r="O122" s="5"/>
       <c r="P122" s="5"/>
     </row>
-    <row r="123" spans="1:16" ht="13">
-      <c r="A123" s="5"/>
-      <c r="B123" s="10"/>
-      <c r="C123" s="5"/>
-      <c r="D123" s="5"/>
-      <c r="E123" s="5"/>
-      <c r="F123" s="5"/>
+    <row r="123" spans="1:16" ht="15">
+      <c r="A123" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B123" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C123" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D123" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E123" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F123" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G123" s="5"/>
       <c r="H123" s="5"/>
       <c r="I123" s="5"/>
@@ -9405,13 +10744,25 @@
       <c r="O123" s="5"/>
       <c r="P123" s="5"/>
     </row>
-    <row r="124" spans="1:16" ht="13">
-      <c r="A124" s="5"/>
-      <c r="B124" s="10"/>
-      <c r="C124" s="5"/>
-      <c r="D124" s="5"/>
-      <c r="E124" s="5"/>
-      <c r="F124" s="5"/>
+    <row r="124" spans="1:16" ht="15">
+      <c r="A124" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="B124" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C124" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D124" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E124" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F124" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G124" s="5"/>
       <c r="H124" s="5"/>
       <c r="I124" s="5"/>
@@ -9423,13 +10774,25 @@
       <c r="O124" s="5"/>
       <c r="P124" s="5"/>
     </row>
-    <row r="125" spans="1:16" ht="13">
-      <c r="A125" s="5"/>
-      <c r="B125" s="10"/>
-      <c r="C125" s="5"/>
-      <c r="D125" s="5"/>
-      <c r="E125" s="5"/>
-      <c r="F125" s="5"/>
+    <row r="125" spans="1:16" ht="15">
+      <c r="A125" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="B125" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C125" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D125" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E125" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F125" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="G125" s="5"/>
       <c r="H125" s="5"/>
       <c r="I125" s="5"/>
@@ -9441,13 +10804,25 @@
       <c r="O125" s="5"/>
       <c r="P125" s="5"/>
     </row>
-    <row r="126" spans="1:16" ht="13">
-      <c r="A126" s="5"/>
-      <c r="B126" s="10"/>
-      <c r="C126" s="5"/>
-      <c r="D126" s="5"/>
-      <c r="E126" s="5"/>
-      <c r="F126" s="5"/>
+    <row r="126" spans="1:16" ht="15">
+      <c r="A126" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="B126" s="29">
+        <v>44532</v>
+      </c>
+      <c r="C126" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D126" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E126" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F126" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="G126" s="5"/>
       <c r="H126" s="5"/>
       <c r="I126" s="5"/>
@@ -9459,13 +10834,25 @@
       <c r="O126" s="5"/>
       <c r="P126" s="5"/>
     </row>
-    <row r="127" spans="1:16" ht="13">
-      <c r="A127" s="5"/>
-      <c r="B127" s="10"/>
-      <c r="C127" s="5"/>
-      <c r="D127" s="5"/>
-      <c r="E127" s="5"/>
-      <c r="F127" s="5"/>
+    <row r="127" spans="1:16" ht="15">
+      <c r="A127" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="B127" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C127" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D127" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="E127" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="F127" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="G127" s="5"/>
       <c r="H127" s="5"/>
       <c r="I127" s="5"/>
@@ -9477,13 +10864,25 @@
       <c r="O127" s="5"/>
       <c r="P127" s="5"/>
     </row>
-    <row r="128" spans="1:16" ht="13">
-      <c r="A128" s="5"/>
-      <c r="B128" s="10"/>
-      <c r="C128" s="5"/>
-      <c r="D128" s="5"/>
-      <c r="E128" s="5"/>
-      <c r="F128" s="5"/>
+    <row r="128" spans="1:16" ht="15">
+      <c r="A128" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="B128" s="29">
+        <v>44531</v>
+      </c>
+      <c r="C128" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D128" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="E128" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="F128" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="G128" s="5"/>
       <c r="H128" s="5"/>
       <c r="I128" s="5"/>
@@ -25193,17 +26592,17 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" prompt="Each sample name must be unique" sqref="A1 A36:A1000" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" prompt="Each sample name must be unique" sqref="A1 A129:A1000" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>COUNTIF($A:$A,"="&amp;A1)  &lt; 2</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B36:B1000" xr:uid="{00000000-0002-0000-0100-000003000000}">
-      <formula1>OR(NOT(ISERROR(DATEVALUE(B36))), AND(ISNUMBER(B36), LEFT(CELL("format", B36))="D"))</formula1>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B129:B1000" xr:uid="{00000000-0002-0000-0100-000003000000}">
+      <formula1>OR(NOT(ISERROR(DATEVALUE(B129))), AND(ISNUMBER(B129), LEFT(CELL("format", B129))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" prompt="Each sample name must be unique" sqref="A2:A35" xr:uid="{11FEE6CA-6C10-F746-A179-C78A01C4B3DC}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" prompt="Each sample name must be unique" sqref="A2:A72 A77:A128" xr:uid="{3984FC27-3A22-004D-9B04-020A46696D65}">
       <formula1>COUNTIF($A:$A,"="&amp;A2)  &lt; 2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B35" xr:uid="{7A931936-BA46-914A-BF7B-252DE2444F3F}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B128" xr:uid="{B5885D27-95E9-F54F-968A-C11973089060}">
       <formula1>OR(NOT(ISERROR(DATEVALUE(B2))), AND(ISNUMBER(B2), LEFT(CELL("format", B2))="D"))</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -25215,15 +26614,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Animal ID must match one from the &quot;Animals&quot; sheet" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
-            <xm:f>Animals!$A$2:$A1034</xm:f>
+            <xm:f>Animals!$A$2:$A1127</xm:f>
           </x14:formula1>
-          <xm:sqref>F36:F1000</xm:sqref>
+          <xm:sqref>F129:F1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Tissues must be from the list on the &quot;Tissues&quot; sheet" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>Tissues!$A$2:$A$36</xm:f>
           </x14:formula1>
-          <xm:sqref>D36:D1000</xm:sqref>
+          <xm:sqref>D129:D1000</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -25318,7 +26717,7 @@
   </sheetPr>
   <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
@@ -25685,7 +27084,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" ht="18">
       <c r="A1" s="15" t="s">
         <v>5</v>
       </c>
@@ -25784,7 +27183,7 @@
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
       <c r="A16" s="5"/>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" ht="18">
       <c r="A17" s="18" t="s">
         <v>92</v>
       </c>

</xml_diff>